<commit_message>
added grade feature and reformat the excel file
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abdul\My Document\Upwork\Projects\Gettech.com - John\Product Pricing\webscraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8D6179-8FD6-421C-9544-4729F90D814E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6465BA-D583-4A71-A5BA-7EFB747E33E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{10FC9091-0F44-4BBE-AA13-75D9C8658F19}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Grade</t>
   </si>
   <si>
@@ -74,13 +71,13 @@
     <t>Margin %</t>
   </si>
   <si>
-    <t xml:space="preserve">Selling_Price </t>
-  </si>
-  <si>
     <t>Cash_Buying_Price</t>
   </si>
   <si>
-    <t>Voucher_Buying_Price</t>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
 </sst>
 </file>
@@ -115,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,14 +137,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -204,21 +195,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -238,21 +214,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -272,6 +233,100 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -280,55 +335,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,111 +707,104 @@
   <dimension ref="B1:P5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="4" max="4" width="10" style="10"/>
-    <col min="5" max="5" width="41.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2"/>
+    <col min="8" max="8" width="41.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1"/>
-    <col min="13" max="13" width="10" style="2"/>
-    <col min="14" max="14" width="10" style="13"/>
-    <col min="15" max="15" width="10" style="10"/>
-    <col min="16" max="16" width="10" style="11"/>
+    <col min="12" max="12" width="10" style="2"/>
+    <col min="13" max="13" width="10" style="1"/>
+    <col min="14" max="14" width="10" style="21"/>
+    <col min="16" max="16" width="10" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:16" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="2:16" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="24"/>
-    </row>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="17"/>
+      <c r="O2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="P2" s="17"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="L4" s="6"/>
       <c r="M4" s="7"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="L5" s="6"/>
       <c r="M5" s="7"/>
+      <c r="O5" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
+  <mergeCells count="6">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="K1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>